<commit_message>
database upgrade, Ryanrent V2
</commit_message>
<xml_diff>
--- a/Shared/Sources/aub_huizenlijst.xlsx
+++ b/Shared/Sources/aub_huizenlijst.xlsx
@@ -4356,4 +4356,271 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId10"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD8216A3BCF59A4CAC1EDC9B65F03F94" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7a5dd83b0615c7ab65f6e497dc3f1a67">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2" xmlns:ns3="7c6541c9-858d-46cc-aee4-1fa681dc1bd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b3083ab368e81f90f854d4b93d60013" ns2:_="" ns3:_="">
+    <xsd:import namespace="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2"/>
+    <xsd:import namespace="7c6541c9-858d-46cc-aee4-1fa681dc1bd6"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="11" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="5bd66242-e0b1-4d5e-a424-ed2be647a714" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="17" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="18" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="21" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7c6541c9-858d-46cc-aee4-1fa681dc1bd6" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="16" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{5de6d577-5e06-4df3-9e53-a11405c55b7c}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="7c6541c9-858d-46cc-aee4-1fa681dc1bd6">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c6541c9-858d-46cc-aee4-1fa681dc1bd6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1B8B65B-90D4-4CFA-B64D-55ACEE3E0EDE}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F540105A-E155-4263-8FF1-0970CB25BEC5}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58A0F90D-F385-44E4-8B91-56BDAB481306}"/>
 </file>
</xml_diff>

<commit_message>
data upgrade relaties linked to verhuur en inhuur
</commit_message>
<xml_diff>
--- a/Shared/Sources/aub_huizenlijst.xlsx
+++ b/Shared/Sources/aub_huizenlijst.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ryanrent.sharepoint.com/sites/RyanRent/Gedeelde documenten/General/01_RyanRent&amp;Co/Aljereau/Eindafrekening Generator/Shared/Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{BBAF9F8C-8115-D145-B462-64EF9272AD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C15A1295-DE63-E84F-BA0D-784450D71A50}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{BBAF9F8C-8115-D145-B462-64EF9272AD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{814579D5-CCDD-F548-BB5C-F01F0E985693}"/>
   <bookViews>
-    <workbookView xWindow="-2220" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{0AA87CA2-DCAE-3845-8A9A-48F9A34B6118}"/>
+    <workbookView xWindow="-2220" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{0AA87CA2-DCAE-3845-8A9A-48F9A34B6118}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="info" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -129,8 +130,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="263">
   <si>
     <t>object_id</t>
   </si>
@@ -916,6 +939,9 @@
   </si>
   <si>
     <t>0286</t>
+  </si>
+  <si>
+    <t>gwe_voorschot</t>
   </si>
 </sst>
 </file>
@@ -926,7 +952,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ &quot;€&quot;\ * #,##0.00000_ ;_ &quot;€&quot;\ * \-#,##0.00000_ ;_ &quot;€&quot;\ * &quot;-&quot;?????_ ;_ @_ "/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1003,6 +1029,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1061,7 +1094,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1106,12 +1139,6 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1139,25 +1166,10 @@
     <xf numFmtId="44" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="1" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1169,6 +1181,36 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1510,8 +1552,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C00335-F73E-E948-90F0-C23178DD6B5A}">
   <dimension ref="A1:AR23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1691,7 +1736,7 @@
       </c>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="40" t="s">
         <v>243</v>
       </c>
       <c r="B2" t="s">
@@ -1791,26 +1836,26 @@
       <c r="AG2" s="17">
         <v>66.36</v>
       </c>
-      <c r="AH2" s="18" t="s">
+      <c r="AH2" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="AI2" s="19">
+      <c r="AI2" s="45">
         <v>115.76</v>
       </c>
-      <c r="AJ2" s="18" t="s">
+      <c r="AJ2" s="44" t="s">
         <v>58</v>
       </c>
       <c r="AK2" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AL2" s="20">
+      <c r="AL2" s="18">
         <v>79</v>
       </c>
       <c r="AM2" s="12" t="s">
         <v>52</v>
       </c>
       <c r="AN2" s="11"/>
-      <c r="AO2" s="21">
+      <c r="AO2" s="19">
         <v>41791</v>
       </c>
       <c r="AP2" t="s">
@@ -1821,7 +1866,7 @@
       </c>
     </row>
     <row r="3" spans="1:44" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="20" t="s">
         <v>244</v>
       </c>
       <c r="B3" t="s">
@@ -1921,20 +1966,20 @@
       <c r="AG3" s="17">
         <v>66.36</v>
       </c>
-      <c r="AH3" s="18"/>
-      <c r="AI3" s="18"/>
-      <c r="AJ3" s="18"/>
+      <c r="AH3" s="44"/>
+      <c r="AI3" s="44"/>
+      <c r="AJ3" s="44"/>
       <c r="AK3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AL3" s="20">
+      <c r="AL3" s="18">
         <v>79</v>
       </c>
       <c r="AM3" s="12" t="s">
         <v>52</v>
       </c>
       <c r="AN3" s="11"/>
-      <c r="AO3" s="21">
+      <c r="AO3" s="19">
         <v>41791</v>
       </c>
       <c r="AP3" t="s">
@@ -1945,7 +1990,7 @@
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="40" t="s">
         <v>245</v>
       </c>
       <c r="B4" t="s">
@@ -1978,13 +2023,13 @@
       <c r="K4" t="s">
         <v>70</v>
       </c>
-      <c r="L4" s="23" t="s">
+      <c r="L4" s="21" t="s">
         <v>71</v>
       </c>
       <c r="M4" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="22">
         <v>6</v>
       </c>
       <c r="O4" s="10">
@@ -1999,7 +2044,7 @@
       <c r="R4" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="25" t="s">
+      <c r="S4" s="23" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="14">
@@ -2008,7 +2053,7 @@
       <c r="U4" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="V4" s="25" t="s">
+      <c r="V4" s="23" t="s">
         <v>54</v>
       </c>
       <c r="W4" s="14">
@@ -2020,7 +2065,7 @@
       <c r="Y4" s="15">
         <v>0.16794000000000001</v>
       </c>
-      <c r="Z4" s="25" t="s">
+      <c r="Z4" s="23" t="s">
         <v>55</v>
       </c>
       <c r="AA4" s="12" t="s">
@@ -2058,22 +2103,22 @@
       <c r="AK4" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AL4" s="20">
+      <c r="AL4" s="18">
         <v>79</v>
       </c>
       <c r="AM4" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="AN4" s="26">
+      <c r="AN4" s="24">
         <v>1200</v>
       </c>
-      <c r="AO4" s="21">
+      <c r="AO4" s="19">
         <v>43466</v>
       </c>
-      <c r="AP4" s="21">
+      <c r="AP4" s="19">
         <v>44196</v>
       </c>
-      <c r="AQ4" s="27" t="s">
+      <c r="AQ4" s="25" t="s">
         <v>75</v>
       </c>
       <c r="AR4" t="s">
@@ -2081,7 +2126,7 @@
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="40" t="s">
         <v>246</v>
       </c>
       <c r="B5" t="s">
@@ -2114,7 +2159,7 @@
       <c r="K5" t="s">
         <v>82</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="L5" s="21" t="s">
         <v>83</v>
       </c>
       <c r="M5" s="10" t="s">
@@ -2135,7 +2180,7 @@
       <c r="R5" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="S5" s="25" t="s">
+      <c r="S5" s="23" t="s">
         <v>54</v>
       </c>
       <c r="T5" s="14">
@@ -2144,7 +2189,7 @@
       <c r="U5" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="V5" s="25" t="s">
+      <c r="V5" s="23" t="s">
         <v>54</v>
       </c>
       <c r="W5" s="14">
@@ -2156,7 +2201,7 @@
       <c r="Y5" s="15">
         <v>0.16794000000000001</v>
       </c>
-      <c r="Z5" s="25" t="s">
+      <c r="Z5" s="23" t="s">
         <v>55</v>
       </c>
       <c r="AA5" s="12" t="s">
@@ -2193,14 +2238,14 @@
       <c r="AK5" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AL5" s="20">
+      <c r="AL5" s="18">
         <v>0</v>
       </c>
       <c r="AM5" s="12"/>
-      <c r="AN5" s="26">
+      <c r="AN5" s="24">
         <v>2300</v>
       </c>
-      <c r="AO5" s="21">
+      <c r="AO5" s="19">
         <v>41239</v>
       </c>
       <c r="AP5" t="s">
@@ -2211,7 +2256,7 @@
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="40" t="s">
         <v>247</v>
       </c>
       <c r="B6" t="s">
@@ -2250,7 +2295,7 @@
       <c r="M6" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="N6" s="24">
+      <c r="N6" s="22">
         <v>8</v>
       </c>
       <c r="O6" s="10">
@@ -2265,7 +2310,7 @@
       <c r="R6" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="S6" s="25" t="s">
+      <c r="S6" s="23" t="s">
         <v>54</v>
       </c>
       <c r="T6" s="14">
@@ -2274,7 +2319,7 @@
       <c r="U6" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="V6" s="25" t="s">
+      <c r="V6" s="23" t="s">
         <v>54</v>
       </c>
       <c r="W6" s="14">
@@ -2286,7 +2331,7 @@
       <c r="Y6" s="15">
         <v>0.16794000000000001</v>
       </c>
-      <c r="Z6" s="25" t="s">
+      <c r="Z6" s="23" t="s">
         <v>55</v>
       </c>
       <c r="AA6" s="12" t="s">
@@ -2323,22 +2368,22 @@
       <c r="AK6" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AL6" s="20">
+      <c r="AL6" s="18">
         <v>79</v>
       </c>
       <c r="AM6" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="AN6" s="26">
+      <c r="AN6" s="24">
         <v>2150</v>
       </c>
-      <c r="AO6" s="21">
+      <c r="AO6" s="19">
         <v>43896</v>
       </c>
-      <c r="AP6" s="21">
+      <c r="AP6" s="19">
         <v>44261</v>
       </c>
-      <c r="AQ6" s="28" t="s">
+      <c r="AQ6" s="26" t="s">
         <v>98</v>
       </c>
       <c r="AR6" t="s">
@@ -2346,7 +2391,7 @@
       </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="40" t="s">
         <v>248</v>
       </c>
       <c r="B7" t="s">
@@ -2400,7 +2445,7 @@
       <c r="R7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="S7" s="25" t="s">
+      <c r="S7" s="23" t="s">
         <v>54</v>
       </c>
       <c r="T7" s="14">
@@ -2458,25 +2503,25 @@
       <c r="AK7" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="AL7" s="20">
+      <c r="AL7" s="18">
         <v>0</v>
       </c>
       <c r="AM7" s="12" t="s">
         <v>52</v>
       </c>
       <c r="AN7" s="11"/>
-      <c r="AO7" s="21">
+      <c r="AO7" s="19">
         <v>41239</v>
       </c>
-      <c r="AP7" s="29">
+      <c r="AP7" s="27">
         <v>44197</v>
       </c>
-      <c r="AQ7" s="30" t="s">
+      <c r="AQ7" s="28" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="40" t="s">
         <v>249</v>
       </c>
       <c r="B8" t="s">
@@ -2503,7 +2548,7 @@
       <c r="I8" t="s">
         <v>120</v>
       </c>
-      <c r="J8" s="31" t="s">
+      <c r="J8" s="29" t="s">
         <v>121</v>
       </c>
       <c r="K8" t="s">
@@ -2515,7 +2560,7 @@
       <c r="M8" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="N8" s="24">
+      <c r="N8" s="22">
         <v>4</v>
       </c>
       <c r="O8" s="10">
@@ -2530,16 +2575,16 @@
       <c r="R8" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="S8" s="25" t="s">
+      <c r="S8" s="23" t="s">
         <v>111</v>
       </c>
       <c r="T8" s="14">
         <v>0</v>
       </c>
-      <c r="U8" s="25" t="s">
+      <c r="U8" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="V8" s="25" t="s">
+      <c r="V8" s="23" t="s">
         <v>111</v>
       </c>
       <c r="W8" s="14">
@@ -2551,10 +2596,10 @@
       <c r="Y8" s="15">
         <v>0</v>
       </c>
-      <c r="Z8" s="25" t="s">
+      <c r="Z8" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="AA8" s="25" t="s">
+      <c r="AA8" s="23" t="s">
         <v>111</v>
       </c>
       <c r="AB8" s="12"/>
@@ -2581,66 +2626,66 @@
       <c r="AK8" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="AL8" s="20">
+      <c r="AL8" s="18">
         <v>0</v>
       </c>
       <c r="AM8" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="AN8" s="26">
+      <c r="AN8" s="24">
         <v>1000</v>
       </c>
-      <c r="AO8" s="21">
+      <c r="AO8" s="19">
         <v>43160</v>
       </c>
       <c r="AP8" t="s">
         <v>128</v>
       </c>
-      <c r="AQ8" s="27" t="s">
+      <c r="AQ8" s="25" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="41" t="s">
         <v>250</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="32">
         <v>41710</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="33">
         <v>119</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="G9" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="I9" s="32" t="s">
+      <c r="I9" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="J9" s="36" t="s">
+      <c r="J9" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="K9" s="32" t="s">
+      <c r="K9" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="L9" s="37" t="s">
+      <c r="L9" s="46" t="s">
         <v>138</v>
       </c>
       <c r="M9" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="N9" s="24">
+      <c r="N9" s="22">
         <v>150</v>
       </c>
       <c r="O9" s="10">
@@ -2658,11 +2703,11 @@
       <c r="S9" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="T9" s="38"/>
+      <c r="T9" s="35"/>
       <c r="U9" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="V9" s="25" t="s">
+      <c r="V9" s="23" t="s">
         <v>54</v>
       </c>
       <c r="W9" s="14">
@@ -2702,69 +2747,69 @@
       <c r="AH9" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="AI9" s="39">
+      <c r="AI9" s="48">
         <v>845.56</v>
       </c>
-      <c r="AJ9" s="18" t="s">
+      <c r="AJ9" s="44" t="s">
         <v>142</v>
       </c>
       <c r="AK9" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AL9" s="20">
+      <c r="AL9" s="18">
         <v>237</v>
       </c>
       <c r="AM9" s="12"/>
       <c r="AN9" s="11"/>
-      <c r="AO9" s="21">
+      <c r="AO9" s="19">
         <v>43591</v>
       </c>
-      <c r="AP9" s="40">
+      <c r="AP9" s="36">
         <v>45396</v>
       </c>
-      <c r="AR9" s="41" t="s">
+      <c r="AR9" s="42" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="41" t="s">
         <v>250</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="32">
         <v>1500</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10" s="33">
         <v>119</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="G10" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="H10" s="32" t="s">
+      <c r="H10" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="I10" s="32" t="s">
+      <c r="I10" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="J10" s="36" t="s">
+      <c r="J10" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="K10" s="32" t="s">
+      <c r="K10" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="L10" s="42"/>
+      <c r="L10" s="47"/>
       <c r="M10" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="N10" s="24"/>
+      <c r="N10" s="22"/>
       <c r="O10" s="10"/>
       <c r="P10" t="s">
         <v>52</v>
@@ -2778,11 +2823,11 @@
       <c r="S10" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="T10" s="38"/>
+      <c r="T10" s="35"/>
       <c r="U10" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="V10" s="25" t="s">
+      <c r="V10" s="23" t="s">
         <v>54</v>
       </c>
       <c r="W10" s="14">
@@ -2797,7 +2842,7 @@
       <c r="Z10" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="AA10" s="25" t="s">
+      <c r="AA10" s="23" t="s">
         <v>140</v>
       </c>
       <c r="AB10" s="12">
@@ -2821,26 +2866,26 @@
       <c r="AH10" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="AI10" s="41"/>
-      <c r="AJ10" s="18"/>
+      <c r="AI10" s="42"/>
+      <c r="AJ10" s="44"/>
       <c r="AK10" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AL10" s="20">
+      <c r="AL10" s="18">
         <v>395</v>
       </c>
       <c r="AM10" s="12"/>
       <c r="AN10" s="11"/>
-      <c r="AO10" s="21">
+      <c r="AO10" s="19">
         <v>43891</v>
       </c>
-      <c r="AP10" s="40">
+      <c r="AP10" s="36">
         <v>45396</v>
       </c>
-      <c r="AR10" s="41"/>
+      <c r="AR10" s="42"/>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="40" t="s">
         <v>251</v>
       </c>
       <c r="B11" t="s">
@@ -2946,16 +2991,16 @@
       <c r="AK11" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AL11" s="20">
+      <c r="AL11" s="18">
         <v>79</v>
       </c>
       <c r="AM11" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="AN11" s="26">
+      <c r="AN11" s="24">
         <v>1750</v>
       </c>
-      <c r="AO11" s="21">
+      <c r="AO11" s="19">
         <v>43079</v>
       </c>
       <c r="AP11" t="s">
@@ -2969,7 +3014,7 @@
       </c>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="40" t="s">
         <v>252</v>
       </c>
       <c r="B12" t="s">
@@ -3023,7 +3068,7 @@
       <c r="R12" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="S12" s="25" t="s">
+      <c r="S12" s="23" t="s">
         <v>54</v>
       </c>
       <c r="T12" s="14">
@@ -3032,7 +3077,7 @@
       <c r="U12" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="V12" s="25" t="s">
+      <c r="V12" s="23" t="s">
         <v>54</v>
       </c>
       <c r="W12" s="14">
@@ -3044,7 +3089,7 @@
       <c r="Y12" s="15">
         <v>0.16794000000000001</v>
       </c>
-      <c r="Z12" s="25" t="s">
+      <c r="Z12" s="23" t="s">
         <v>55</v>
       </c>
       <c r="AA12" s="12" t="s">
@@ -3082,14 +3127,14 @@
       <c r="AK12" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AL12" s="20">
+      <c r="AL12" s="18">
         <v>79</v>
       </c>
       <c r="AM12" s="12" t="s">
         <v>52</v>
       </c>
       <c r="AN12" s="11"/>
-      <c r="AO12" s="21">
+      <c r="AO12" s="19">
         <v>41239</v>
       </c>
       <c r="AP12" t="s">
@@ -3097,7 +3142,7 @@
       </c>
     </row>
     <row r="13" spans="1:44" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="20" t="s">
         <v>253</v>
       </c>
       <c r="B13" t="s">
@@ -3145,18 +3190,18 @@
       <c r="R13" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="S13" s="25"/>
+      <c r="S13" s="23"/>
       <c r="T13" s="14"/>
       <c r="U13" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="V13" s="25" t="s">
+      <c r="V13" s="23" t="s">
         <v>110</v>
       </c>
       <c r="W13" s="14"/>
       <c r="X13" s="15"/>
       <c r="Y13" s="15"/>
-      <c r="Z13" s="25"/>
+      <c r="Z13" s="23"/>
       <c r="AA13" s="12"/>
       <c r="AB13" s="12"/>
       <c r="AC13" s="16">
@@ -3179,7 +3224,7 @@
       <c r="AK13" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AL13" s="20">
+      <c r="AL13" s="18">
         <v>79</v>
       </c>
       <c r="AM13" s="12" t="s">
@@ -3188,12 +3233,12 @@
       <c r="AN13" s="11">
         <v>3600</v>
       </c>
-      <c r="AO13" s="21">
+      <c r="AO13" s="19">
         <v>45659</v>
       </c>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="40" t="s">
         <v>254</v>
       </c>
       <c r="B14" t="s">
@@ -3226,7 +3271,7 @@
       <c r="K14" t="s">
         <v>178</v>
       </c>
-      <c r="L14" s="23" t="s">
+      <c r="L14" s="21" t="s">
         <v>179</v>
       </c>
       <c r="M14" s="10" t="s">
@@ -3299,12 +3344,12 @@
       <c r="AK14" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AL14" s="20">
+      <c r="AL14" s="18">
         <v>79</v>
       </c>
       <c r="AM14" s="12"/>
       <c r="AN14" s="11"/>
-      <c r="AO14" s="40">
+      <c r="AO14" s="36">
         <v>42826</v>
       </c>
       <c r="AP14" t="s">
@@ -3312,7 +3357,7 @@
       </c>
     </row>
     <row r="15" spans="1:44" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="20" t="s">
         <v>255</v>
       </c>
       <c r="B15" t="s">
@@ -3345,7 +3390,7 @@
       <c r="K15" t="s">
         <v>189</v>
       </c>
-      <c r="L15" s="23" t="s">
+      <c r="L15" s="21" t="s">
         <v>190</v>
       </c>
       <c r="M15" s="10" t="s">
@@ -3366,7 +3411,7 @@
       <c r="R15" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="S15" s="25" t="s">
+      <c r="S15" s="23" t="s">
         <v>54</v>
       </c>
       <c r="T15" s="14">
@@ -3424,17 +3469,17 @@
         <v>192</v>
       </c>
       <c r="AK15" s="10"/>
-      <c r="AL15" s="20">
+      <c r="AL15" s="18">
         <v>79</v>
       </c>
       <c r="AM15" s="12"/>
       <c r="AN15" s="11"/>
-      <c r="AO15" s="40">
+      <c r="AO15" s="36">
         <v>44256</v>
       </c>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>256</v>
       </c>
       <c r="B16" t="s">
@@ -3467,16 +3512,16 @@
       <c r="K16" t="s">
         <v>199</v>
       </c>
-      <c r="L16" s="23" t="s">
+      <c r="L16" s="21" t="s">
         <v>200</v>
       </c>
       <c r="M16" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="N16" s="24"/>
+      <c r="N16" s="22"/>
       <c r="O16" s="10"/>
       <c r="R16" s="12"/>
-      <c r="S16" s="25"/>
+      <c r="S16" s="23"/>
       <c r="T16" s="14"/>
       <c r="U16" s="12"/>
       <c r="V16" s="12"/>
@@ -3495,17 +3540,17 @@
       <c r="AI16" s="43">
         <v>138.19999999999999</v>
       </c>
-      <c r="AJ16" s="18" t="s">
+      <c r="AJ16" s="44" t="s">
         <v>202</v>
       </c>
       <c r="AK16" s="10"/>
-      <c r="AL16" s="20"/>
+      <c r="AL16" s="18"/>
       <c r="AM16" s="12"/>
       <c r="AN16" s="11"/>
-      <c r="AO16" s="40">
+      <c r="AO16" s="36">
         <v>45231</v>
       </c>
-      <c r="AP16" s="40">
+      <c r="AP16" s="36">
         <v>45961</v>
       </c>
       <c r="AQ16" t="s">
@@ -3513,7 +3558,7 @@
       </c>
     </row>
     <row r="17" spans="1:44" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="20" t="s">
         <v>257</v>
       </c>
       <c r="B17" t="s">
@@ -3546,7 +3591,7 @@
       <c r="K17" t="s">
         <v>199</v>
       </c>
-      <c r="L17" s="23" t="s">
+      <c r="L17" s="21" t="s">
         <v>200</v>
       </c>
       <c r="M17" s="10" t="s">
@@ -3555,7 +3600,7 @@
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
       <c r="R17" s="12"/>
-      <c r="S17" s="25"/>
+      <c r="S17" s="23"/>
       <c r="T17" s="14"/>
       <c r="U17" s="12"/>
       <c r="V17" s="12"/>
@@ -3575,16 +3620,16 @@
       <c r="AH17" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="AI17" s="41"/>
-      <c r="AJ17" s="18"/>
+      <c r="AI17" s="42"/>
+      <c r="AJ17" s="44"/>
       <c r="AK17" s="10"/>
-      <c r="AL17" s="20"/>
+      <c r="AL17" s="18"/>
       <c r="AM17" s="12"/>
       <c r="AN17" s="11"/>
-      <c r="AO17" s="40">
+      <c r="AO17" s="36">
         <v>45108</v>
       </c>
-      <c r="AP17" s="40">
+      <c r="AP17" s="36">
         <v>46568</v>
       </c>
       <c r="AQ17" t="s">
@@ -3595,7 +3640,7 @@
       </c>
     </row>
     <row r="18" spans="1:44" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="20" t="s">
         <v>258</v>
       </c>
       <c r="B18" t="s">
@@ -3622,7 +3667,7 @@
       <c r="I18" t="s">
         <v>210</v>
       </c>
-      <c r="J18" s="31" t="s">
+      <c r="J18" s="29" t="s">
         <v>211</v>
       </c>
       <c r="K18" t="s">
@@ -3646,7 +3691,7 @@
       <c r="R18" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="S18" s="25" t="s">
+      <c r="S18" s="23" t="s">
         <v>54</v>
       </c>
       <c r="T18" s="14">
@@ -3655,7 +3700,7 @@
       <c r="U18" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="V18" s="25" t="s">
+      <c r="V18" s="23" t="s">
         <v>54</v>
       </c>
       <c r="W18" s="14">
@@ -3667,7 +3712,7 @@
       <c r="Y18" s="15">
         <v>0.24836</v>
       </c>
-      <c r="Z18" s="25" t="s">
+      <c r="Z18" s="23" t="s">
         <v>55</v>
       </c>
       <c r="AA18" s="12" t="s">
@@ -3697,17 +3742,17 @@
       </c>
       <c r="AJ18" s="10"/>
       <c r="AK18" s="10"/>
-      <c r="AL18" s="20"/>
+      <c r="AL18" s="18"/>
       <c r="AM18" s="12" t="s">
         <v>52</v>
       </c>
       <c r="AN18" s="11">
         <v>1300</v>
       </c>
-      <c r="AO18" s="21">
+      <c r="AO18" s="19">
         <v>44927</v>
       </c>
-      <c r="AP18" s="40">
+      <c r="AP18" s="36">
         <v>45291</v>
       </c>
       <c r="AQ18" t="s">
@@ -3715,7 +3760,7 @@
       </c>
     </row>
     <row r="19" spans="1:44" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="20" t="s">
         <v>259</v>
       </c>
       <c r="B19" t="s">
@@ -3742,7 +3787,7 @@
       <c r="I19" t="s">
         <v>210</v>
       </c>
-      <c r="J19" s="31" t="s">
+      <c r="J19" s="29" t="s">
         <v>211</v>
       </c>
       <c r="K19" t="s">
@@ -3766,7 +3811,7 @@
       <c r="R19" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="S19" s="25" t="s">
+      <c r="S19" s="23" t="s">
         <v>54</v>
       </c>
       <c r="T19" s="14">
@@ -3775,7 +3820,7 @@
       <c r="U19" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="V19" s="25" t="s">
+      <c r="V19" s="23" t="s">
         <v>54</v>
       </c>
       <c r="W19" s="14">
@@ -3787,7 +3832,7 @@
       <c r="Y19" s="15">
         <v>0.24836</v>
       </c>
-      <c r="Z19" s="25" t="s">
+      <c r="Z19" s="23" t="s">
         <v>55</v>
       </c>
       <c r="AA19" s="12" t="s">
@@ -3817,17 +3862,17 @@
       </c>
       <c r="AJ19" s="10"/>
       <c r="AK19" s="10"/>
-      <c r="AL19" s="20"/>
+      <c r="AL19" s="18"/>
       <c r="AM19" s="12" t="s">
         <v>52</v>
       </c>
       <c r="AN19" s="11">
         <v>1950</v>
       </c>
-      <c r="AO19" s="21">
+      <c r="AO19" s="19">
         <v>44927</v>
       </c>
-      <c r="AP19" s="40">
+      <c r="AP19" s="36">
         <v>45291</v>
       </c>
       <c r="AQ19" t="s">
@@ -3835,7 +3880,7 @@
       </c>
     </row>
     <row r="20" spans="1:44" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="20" t="s">
         <v>260</v>
       </c>
       <c r="B20" t="s">
@@ -3874,7 +3919,7 @@
       <c r="M20" t="s">
         <v>223</v>
       </c>
-      <c r="N20" s="24">
+      <c r="N20" s="22">
         <v>4</v>
       </c>
       <c r="O20" s="10">
@@ -3889,7 +3934,7 @@
       <c r="R20" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="S20" s="25" t="s">
+      <c r="S20" s="23" t="s">
         <v>224</v>
       </c>
       <c r="T20" s="14">
@@ -3898,7 +3943,7 @@
       <c r="U20" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="V20" s="25" t="s">
+      <c r="V20" s="23" t="s">
         <v>224</v>
       </c>
       <c r="W20" s="14">
@@ -3910,7 +3955,7 @@
       <c r="Y20" s="15">
         <v>4.2009999999999999E-2</v>
       </c>
-      <c r="Z20" s="25" t="s">
+      <c r="Z20" s="23" t="s">
         <v>55</v>
       </c>
       <c r="AA20" s="12" t="s">
@@ -3937,7 +3982,7 @@
       <c r="AH20" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="AI20" s="44">
+      <c r="AI20" s="37">
         <f>166.43/3</f>
         <v>55.476666666666667</v>
       </c>
@@ -3947,23 +3992,23 @@
       <c r="AK20" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="AL20" s="20">
+      <c r="AL20" s="18">
         <v>0</v>
       </c>
       <c r="AM20" s="12"/>
       <c r="AN20" s="11"/>
-      <c r="AO20" s="29">
+      <c r="AO20" s="27">
         <v>43600</v>
       </c>
-      <c r="AP20" s="29">
+      <c r="AP20" s="27">
         <v>44695</v>
       </c>
-      <c r="AQ20" s="27" t="s">
+      <c r="AQ20" s="25" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="40" t="s">
         <v>261</v>
       </c>
       <c r="B21" t="s">
@@ -4017,7 +4062,7 @@
       <c r="R21" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="S21" s="25" t="s">
+      <c r="S21" s="23" t="s">
         <v>54</v>
       </c>
       <c r="T21" s="14">
@@ -4026,7 +4071,7 @@
       <c r="U21" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="V21" s="25" t="s">
+      <c r="V21" s="23" t="s">
         <v>54</v>
       </c>
       <c r="W21" s="14">
@@ -4038,7 +4083,7 @@
       <c r="Y21" s="15">
         <v>0.16794000000000001</v>
       </c>
-      <c r="Z21" s="25" t="s">
+      <c r="Z21" s="23" t="s">
         <v>55</v>
       </c>
       <c r="AA21" s="12" t="s">
@@ -4076,14 +4121,14 @@
       <c r="AK21" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AL21" s="20">
+      <c r="AL21" s="18">
         <v>79</v>
       </c>
       <c r="AM21" s="12"/>
-      <c r="AN21" s="26">
+      <c r="AN21" s="24">
         <v>1400</v>
       </c>
-      <c r="AO21" s="21">
+      <c r="AO21" s="19">
         <v>41239</v>
       </c>
       <c r="AP21" t="s">
@@ -4091,7 +4136,7 @@
       </c>
     </row>
     <row r="22" spans="1:44" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="20" t="s">
         <v>235</v>
       </c>
       <c r="B22" t="s">
@@ -4118,7 +4163,7 @@
       <c r="I22" t="s">
         <v>217</v>
       </c>
-      <c r="J22" s="31" t="s">
+      <c r="J22" s="29" t="s">
         <v>48</v>
       </c>
       <c r="K22" t="s">
@@ -4166,19 +4211,19 @@
       <c r="Y22" s="15">
         <v>0</v>
       </c>
-      <c r="Z22" s="25" t="s">
+      <c r="Z22" s="23" t="s">
         <v>55</v>
       </c>
       <c r="AA22" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="AB22" s="45">
+      <c r="AB22" s="38">
         <v>5</v>
       </c>
-      <c r="AC22" s="46">
+      <c r="AC22" s="39">
         <v>44197</v>
       </c>
-      <c r="AD22" s="46">
+      <c r="AD22" s="39">
         <v>46022</v>
       </c>
       <c r="AE22" s="17">
@@ -4196,23 +4241,23 @@
       </c>
       <c r="AJ22" s="10"/>
       <c r="AK22" s="10"/>
-      <c r="AL22" s="20">
+      <c r="AL22" s="18">
         <v>0</v>
       </c>
       <c r="AM22" s="12"/>
       <c r="AN22" s="11"/>
-      <c r="AO22" s="21">
+      <c r="AO22" s="19">
         <v>44927</v>
       </c>
-      <c r="AP22" s="40">
+      <c r="AP22" s="36">
         <v>46022</v>
       </c>
-      <c r="AR22" s="41" t="s">
+      <c r="AR22" s="42" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="23" spans="1:44" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="20" t="s">
         <v>241</v>
       </c>
       <c r="B23" t="s">
@@ -4239,7 +4284,7 @@
       <c r="I23" t="s">
         <v>217</v>
       </c>
-      <c r="J23" s="31" t="s">
+      <c r="J23" s="29" t="s">
         <v>48</v>
       </c>
       <c r="K23" t="s">
@@ -4287,19 +4332,19 @@
       <c r="Y23" s="15">
         <v>0</v>
       </c>
-      <c r="Z23" s="25" t="s">
+      <c r="Z23" s="23" t="s">
         <v>55</v>
       </c>
       <c r="AA23" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="AB23" s="45">
+      <c r="AB23" s="38">
         <v>5</v>
       </c>
-      <c r="AC23" s="46">
+      <c r="AC23" s="39">
         <v>44197</v>
       </c>
-      <c r="AD23" s="46">
+      <c r="AD23" s="39">
         <v>46022</v>
       </c>
       <c r="AE23" s="17">
@@ -4312,35 +4357,35 @@
         <v>0</v>
       </c>
       <c r="AH23" s="10"/>
-      <c r="AI23" s="41"/>
+      <c r="AI23" s="42"/>
       <c r="AJ23" s="10"/>
       <c r="AK23" s="10"/>
-      <c r="AL23" s="20">
+      <c r="AL23" s="18">
         <v>0</v>
       </c>
       <c r="AM23" s="12"/>
       <c r="AN23" s="11"/>
-      <c r="AO23" s="21">
+      <c r="AO23" s="19">
         <v>44927</v>
       </c>
-      <c r="AP23" s="40">
+      <c r="AP23" s="36">
         <v>46022</v>
       </c>
-      <c r="AR23" s="41"/>
+      <c r="AR23" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="AI16:AI17"/>
-    <mergeCell ref="AJ16:AJ17"/>
-    <mergeCell ref="AI22:AI23"/>
-    <mergeCell ref="AR22:AR23"/>
     <mergeCell ref="AH2:AH3"/>
     <mergeCell ref="AI2:AI3"/>
     <mergeCell ref="AJ2:AJ3"/>
     <mergeCell ref="L9:L10"/>
     <mergeCell ref="AI9:AI10"/>
     <mergeCell ref="AJ9:AJ10"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="AI16:AI17"/>
+    <mergeCell ref="AJ16:AJ17"/>
+    <mergeCell ref="AI22:AI23"/>
+    <mergeCell ref="AR22:AR23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L15" r:id="rId1" display="info@jsvink.nl" xr:uid="{9956C1C6-45AC-BC42-ACAB-E6316502D871}"/>
@@ -4354,13 +4399,975 @@
     <hyperlink ref="L13" r:id="rId9" xr:uid="{22A541D5-1F2A-354A-8FB6-F8B7D4A676AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId10"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A303D4ED-CBB7-804E-AA05-5F320B473A7B}">
+  <dimension ref="A1:J23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="50.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="49">
+        <v>280</v>
+      </c>
+      <c r="B2" cm="1">
+        <f t="array" ref="B2">_xlfn.XLOOKUP($A2,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>122.42000000000002</v>
+      </c>
+      <c r="C2" t="str" cm="1">
+        <f t="array" ref="C2">_xlfn.XLOOKUP($A2,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>M. Nottet</v>
+      </c>
+      <c r="D2" t="str" cm="1">
+        <f t="array" ref="D2">_xlfn.XLOOKUP($A2,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>M. Nottet</v>
+      </c>
+      <c r="E2" t="str" cm="1">
+        <f t="array" ref="E2">_xlfn.XLOOKUP($A2,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Kapittelland 16</v>
+      </c>
+      <c r="F2" t="str" cm="1">
+        <f t="array" ref="F2">_xlfn.XLOOKUP($A2,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>3151 ZB</v>
+      </c>
+      <c r="G2" t="str" cm="1">
+        <f t="array" ref="G2">_xlfn.XLOOKUP($A2,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Hoek van Holland</v>
+      </c>
+      <c r="H2" t="str" cm="1">
+        <f t="array" ref="H2">_xlfn.XLOOKUP($A2,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-50502637</v>
+      </c>
+      <c r="I2" t="str" cm="1">
+        <f t="array" ref="I2">_xlfn.XLOOKUP($A2,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>mnottet@caiway.nl</v>
+      </c>
+      <c r="J2" t="str" cm="1">
+        <f t="array" ref="J2">_xlfn.XLOOKUP($A2,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL60RABO0323282903</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="50">
+        <v>281</v>
+      </c>
+      <c r="B3" cm="1">
+        <f t="array" ref="B3">_xlfn.XLOOKUP($A3,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>261.87</v>
+      </c>
+      <c r="C3" t="str" cm="1">
+        <f t="array" ref="C3">_xlfn.XLOOKUP($A3,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>M. Nottet</v>
+      </c>
+      <c r="D3" t="str" cm="1">
+        <f t="array" ref="D3">_xlfn.XLOOKUP($A3,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>M. Nottet</v>
+      </c>
+      <c r="E3" t="str" cm="1">
+        <f t="array" ref="E3">_xlfn.XLOOKUP($A3,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Kapittelland 16</v>
+      </c>
+      <c r="F3" t="str" cm="1">
+        <f t="array" ref="F3">_xlfn.XLOOKUP($A3,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>3151 ZB</v>
+      </c>
+      <c r="G3" t="str" cm="1">
+        <f t="array" ref="G3">_xlfn.XLOOKUP($A3,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Hoek van Holland</v>
+      </c>
+      <c r="H3" t="str" cm="1">
+        <f t="array" ref="H3">_xlfn.XLOOKUP($A3,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-50502637</v>
+      </c>
+      <c r="I3" t="str" cm="1">
+        <f t="array" ref="I3">_xlfn.XLOOKUP($A3,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>mnottet@caiway.nl</v>
+      </c>
+      <c r="J3" t="str" cm="1">
+        <f t="array" ref="J3">_xlfn.XLOOKUP($A3,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL60RABO0323282903</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="49">
+        <v>276</v>
+      </c>
+      <c r="B4" cm="1">
+        <f t="array" ref="B4">_xlfn.XLOOKUP($A4,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>589.59</v>
+      </c>
+      <c r="C4" t="str" cm="1">
+        <f t="array" ref="C4">_xlfn.XLOOKUP($A4,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>P. van den Berg</v>
+      </c>
+      <c r="D4" t="str" cm="1">
+        <f t="array" ref="D4">_xlfn.XLOOKUP($A4,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>Piet van den Berg</v>
+      </c>
+      <c r="E4" t="str" cm="1">
+        <f t="array" ref="E4">_xlfn.XLOOKUP($A4,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Burgemeester Cramerlaan 17</v>
+      </c>
+      <c r="F4" t="str" cm="1">
+        <f t="array" ref="F4">_xlfn.XLOOKUP($A4,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>2678 AL</v>
+      </c>
+      <c r="G4" t="str" cm="1">
+        <f t="array" ref="G4">_xlfn.XLOOKUP($A4,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>De Lier</v>
+      </c>
+      <c r="H4" t="str" cm="1">
+        <f t="array" ref="H4">_xlfn.XLOOKUP($A4,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-38765032</v>
+      </c>
+      <c r="I4" t="str" cm="1">
+        <f t="array" ref="I4">_xlfn.XLOOKUP($A4,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>info@vandenbergdelier.nl</v>
+      </c>
+      <c r="J4" t="str" cm="1">
+        <f t="array" ref="J4">_xlfn.XLOOKUP($A4,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL29ABNA0472271989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="49">
+        <v>275</v>
+      </c>
+      <c r="B5" cm="1">
+        <f t="array" ref="B5">_xlfn.XLOOKUP($A5,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>902.34000000000015</v>
+      </c>
+      <c r="C5" t="str" cm="1">
+        <f t="array" ref="C5">_xlfn.XLOOKUP($A5,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>K. Zuidgeest</v>
+      </c>
+      <c r="D5" t="str" cm="1">
+        <f t="array" ref="D5">_xlfn.XLOOKUP($A5,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>K. Zuidgeest</v>
+      </c>
+      <c r="E5" t="str" cm="1">
+        <f t="array" ref="E5">_xlfn.XLOOKUP($A5,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Oudecampsweg 7</v>
+      </c>
+      <c r="F5" t="str" cm="1">
+        <f t="array" ref="F5">_xlfn.XLOOKUP($A5,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>2678 NN</v>
+      </c>
+      <c r="G5" t="str" cm="1">
+        <f t="array" ref="G5">_xlfn.XLOOKUP($A5,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>De Lier</v>
+      </c>
+      <c r="H5" t="str" cm="1">
+        <f t="array" ref="H5">_xlfn.XLOOKUP($A5,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-26146636</v>
+      </c>
+      <c r="I5" t="str" cm="1">
+        <f t="array" ref="I5">_xlfn.XLOOKUP($A5,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v xml:space="preserve">KoosZuidgeest@zuidkoop.nl / k.zuidgeest@hetnet.nl </v>
+      </c>
+      <c r="J5" t="str" cm="1">
+        <f t="array" ref="J5">_xlfn.XLOOKUP($A5,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL05RABO0336208367</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="49">
+        <v>273</v>
+      </c>
+      <c r="B6" cm="1">
+        <f t="array" ref="B6">_xlfn.XLOOKUP($A6,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>388.9</v>
+      </c>
+      <c r="C6" t="str" cm="1">
+        <f t="array" ref="C6">_xlfn.XLOOKUP($A6,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>P.H. Jagt</v>
+      </c>
+      <c r="D6" t="str" cm="1">
+        <f t="array" ref="D6">_xlfn.XLOOKUP($A6,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>Peter Jagt</v>
+      </c>
+      <c r="E6" t="str" cm="1">
+        <f t="array" ref="E6">_xlfn.XLOOKUP($A6,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Haakweg 33</v>
+      </c>
+      <c r="F6" t="str" cm="1">
+        <f t="array" ref="F6">_xlfn.XLOOKUP($A6,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>3151 XD</v>
+      </c>
+      <c r="G6" t="str" cm="1">
+        <f t="array" ref="G6">_xlfn.XLOOKUP($A6,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Hoek van Holland</v>
+      </c>
+      <c r="H6" t="str" cm="1">
+        <f t="array" ref="H6">_xlfn.XLOOKUP($A6,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-51609632</v>
+      </c>
+      <c r="I6" t="str" cm="1">
+        <f t="array" ref="I6">_xlfn.XLOOKUP($A6,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>peter@westhoekmakelaars.nl</v>
+      </c>
+      <c r="J6" t="str" cm="1">
+        <f t="array" ref="J6">_xlfn.XLOOKUP($A6,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL60KNAB0257738010</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="49">
+        <v>279</v>
+      </c>
+      <c r="B7" cm="1">
+        <f t="array" ref="B7">_xlfn.XLOOKUP($A7,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>429.36000000000013</v>
+      </c>
+      <c r="C7" t="str" cm="1">
+        <f t="array" ref="C7">_xlfn.XLOOKUP($A7,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>v.o.f. J.C. Mulder</v>
+      </c>
+      <c r="D7" t="str" cm="1">
+        <f t="array" ref="D7">_xlfn.XLOOKUP($A7,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>Jan Mulder</v>
+      </c>
+      <c r="E7" t="str" cm="1">
+        <f t="array" ref="E7">_xlfn.XLOOKUP($A7,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Nieuwe Tuinen 7B</v>
+      </c>
+      <c r="F7" t="str" cm="1">
+        <f t="array" ref="F7">_xlfn.XLOOKUP($A7,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>2675 SE</v>
+      </c>
+      <c r="G7" t="str" cm="1">
+        <f t="array" ref="G7">_xlfn.XLOOKUP($A7,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Honselersdijk</v>
+      </c>
+      <c r="H7" t="str" cm="1">
+        <f t="array" ref="H7">_xlfn.XLOOKUP($A7,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-53690859</v>
+      </c>
+      <c r="I7" t="str" cm="1">
+        <f t="array" ref="I7">_xlfn.XLOOKUP($A7,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>janmul54@gmail.com</v>
+      </c>
+      <c r="J7" t="str" cm="1">
+        <f t="array" ref="J7">_xlfn.XLOOKUP($A7,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL08RABO0343659077</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="49">
+        <v>274</v>
+      </c>
+      <c r="B8" cm="1">
+        <f t="array" ref="B8">_xlfn.XLOOKUP($A8,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>0</v>
+      </c>
+      <c r="C8" t="str" cm="1">
+        <f t="array" ref="C8">_xlfn.XLOOKUP($A8,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>De Rembrandt B.V.</v>
+      </c>
+      <c r="D8" t="str" cm="1">
+        <f t="array" ref="D8">_xlfn.XLOOKUP($A8,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>Flip van Adrichem</v>
+      </c>
+      <c r="E8" t="str" cm="1">
+        <f t="array" ref="E8">_xlfn.XLOOKUP($A8,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Langestraat 48</v>
+      </c>
+      <c r="F8" t="str" cm="1">
+        <f t="array" ref="F8">_xlfn.XLOOKUP($A8,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>2691 BH</v>
+      </c>
+      <c r="G8" t="str" cm="1">
+        <f t="array" ref="G8">_xlfn.XLOOKUP($A8,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>s-Gravenzande</v>
+      </c>
+      <c r="H8" t="str" cm="1">
+        <f t="array" ref="H8">_xlfn.XLOOKUP($A8,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-41372342</v>
+      </c>
+      <c r="I8" t="str" cm="1">
+        <f t="array" ref="I8">_xlfn.XLOOKUP($A8,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>flip@eetcafedewitte.nl</v>
+      </c>
+      <c r="J8" t="str" cm="1">
+        <f t="array" ref="J8">_xlfn.XLOOKUP($A8,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL21RABO0156104105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="51">
+        <v>291</v>
+      </c>
+      <c r="B9" cm="1">
+        <f t="array" ref="B9">_xlfn.XLOOKUP($A9,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>13978.5</v>
+      </c>
+      <c r="C9" t="str" cm="1">
+        <f t="array" ref="C9">_xlfn.XLOOKUP($A9,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>Lammertink Projecten B.V.</v>
+      </c>
+      <c r="D9" t="str" cm="1">
+        <f t="array" ref="D9">_xlfn.XLOOKUP($A9,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>Hans Lammertink</v>
+      </c>
+      <c r="E9" t="str" cm="1">
+        <f t="array" ref="E9">_xlfn.XLOOKUP($A9,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Schietlood 2</v>
+      </c>
+      <c r="F9" t="str" cm="1">
+        <f t="array" ref="F9">_xlfn.XLOOKUP($A9,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>2495 AN</v>
+      </c>
+      <c r="G9" t="str" cm="1">
+        <f t="array" ref="G9">_xlfn.XLOOKUP($A9,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Den Haag</v>
+      </c>
+      <c r="H9" t="str" cm="1">
+        <f t="array" ref="H9">_xlfn.XLOOKUP($A9,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v xml:space="preserve">085-2739900 </v>
+      </c>
+      <c r="I9" t="str" cm="1">
+        <f t="array" ref="I9">_xlfn.XLOOKUP($A9,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>Dennis Baak 06-24313837 (schoonzoon) / dbaak@l-groep.nl</v>
+      </c>
+      <c r="J9" t="str" cm="1">
+        <f t="array" ref="J9">_xlfn.XLOOKUP($A9,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL83INGB0677182783</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="51">
+        <v>291</v>
+      </c>
+      <c r="B10" cm="1">
+        <f t="array" ref="B10">_xlfn.XLOOKUP($A10,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>13978.5</v>
+      </c>
+      <c r="C10" t="str" cm="1">
+        <f t="array" ref="C10">_xlfn.XLOOKUP($A10,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>Lammertink Projecten B.V.</v>
+      </c>
+      <c r="D10" t="str" cm="1">
+        <f t="array" ref="D10">_xlfn.XLOOKUP($A10,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>Hans Lammertink</v>
+      </c>
+      <c r="E10" t="str" cm="1">
+        <f t="array" ref="E10">_xlfn.XLOOKUP($A10,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Schietlood 2</v>
+      </c>
+      <c r="F10" t="str" cm="1">
+        <f t="array" ref="F10">_xlfn.XLOOKUP($A10,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>2495 AN</v>
+      </c>
+      <c r="G10" t="str" cm="1">
+        <f t="array" ref="G10">_xlfn.XLOOKUP($A10,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Den Haag</v>
+      </c>
+      <c r="H10" t="str" cm="1">
+        <f t="array" ref="H10">_xlfn.XLOOKUP($A10,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v xml:space="preserve">085-2739900 </v>
+      </c>
+      <c r="I10" t="str" cm="1">
+        <f t="array" ref="I10">_xlfn.XLOOKUP($A10,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>Dennis Baak 06-24313837 (schoonzoon) / dbaak@l-groep.nl</v>
+      </c>
+      <c r="J10" t="str" cm="1">
+        <f t="array" ref="J10">_xlfn.XLOOKUP($A10,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL83INGB0677182783</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="49">
+        <v>278</v>
+      </c>
+      <c r="B11" cm="1">
+        <f t="array" ref="B11">_xlfn.XLOOKUP($A11,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>0</v>
+      </c>
+      <c r="C11" t="str" cm="1">
+        <f t="array" ref="C11">_xlfn.XLOOKUP($A11,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>G. Hofland</v>
+      </c>
+      <c r="D11" t="str" cm="1">
+        <f t="array" ref="D11">_xlfn.XLOOKUP($A11,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>Goos Hofland</v>
+      </c>
+      <c r="E11" t="str" cm="1">
+        <f t="array" ref="E11">_xlfn.XLOOKUP($A11,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Lange Broekweg 46</v>
+      </c>
+      <c r="F11" t="str" cm="1">
+        <f t="array" ref="F11">_xlfn.XLOOKUP($A11,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>2671 DV</v>
+      </c>
+      <c r="G11" t="str" cm="1">
+        <f t="array" ref="G11">_xlfn.XLOOKUP($A11,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Naaldwijk</v>
+      </c>
+      <c r="H11" t="str" cm="1">
+        <f t="array" ref="H11">_xlfn.XLOOKUP($A11,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>0174-625887</v>
+      </c>
+      <c r="I11" t="str" cm="1">
+        <f t="array" ref="I11">_xlfn.XLOOKUP($A11,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>goos@hoflandfloweringplants.nl</v>
+      </c>
+      <c r="J11" t="str" cm="1">
+        <f t="array" ref="J11">_xlfn.XLOOKUP($A11,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL27RABO0343661063</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="49">
+        <v>284</v>
+      </c>
+      <c r="B12" cm="1">
+        <f t="array" ref="B12">_xlfn.XLOOKUP($A12,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>609.67000000000007</v>
+      </c>
+      <c r="C12" t="str" cm="1">
+        <f t="array" ref="C12">_xlfn.XLOOKUP($A12,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>M.J.W. van den Enden &amp; B.M. van den Enden</v>
+      </c>
+      <c r="D12" t="str" cm="1">
+        <f t="array" ref="D12">_xlfn.XLOOKUP($A12,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>Barbara van den Enden</v>
+      </c>
+      <c r="E12" t="str" cm="1">
+        <f t="array" ref="E12">_xlfn.XLOOKUP($A12,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Bospolder 4a</v>
+      </c>
+      <c r="F12" t="str" cm="1">
+        <f t="array" ref="F12">_xlfn.XLOOKUP($A12,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>2675 BL</v>
+      </c>
+      <c r="G12" t="str" cm="1">
+        <f t="array" ref="G12">_xlfn.XLOOKUP($A12,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Honselersdijk</v>
+      </c>
+      <c r="H12" t="str" cm="1">
+        <f t="array" ref="H12">_xlfn.XLOOKUP($A12,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-51611737 Barbara / 06-54398790 Maup</v>
+      </c>
+      <c r="I12" t="str" cm="1">
+        <f t="array" ref="I12">_xlfn.XLOOKUP($A12,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>endem3@caiway.nl</v>
+      </c>
+      <c r="J12" t="str" cm="1">
+        <f t="array" ref="J12">_xlfn.XLOOKUP($A12,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL81INGB0112509347</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="50">
+        <v>335</v>
+      </c>
+      <c r="B13" cm="1">
+        <f t="array" ref="B13">_xlfn.XLOOKUP($A13,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>200</v>
+      </c>
+      <c r="C13" t="str" cm="1">
+        <f t="array" ref="C13">_xlfn.XLOOKUP($A13,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>M.J.W. van den Enden &amp; B.M. van den Enden</v>
+      </c>
+      <c r="D13" t="str" cm="1">
+        <f t="array" ref="D13">_xlfn.XLOOKUP($A13,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>Barbara van den Enden</v>
+      </c>
+      <c r="E13" t="str" cm="1">
+        <f t="array" ref="E13">_xlfn.XLOOKUP($A13,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Bospolder 4a</v>
+      </c>
+      <c r="F13" t="str" cm="1">
+        <f t="array" ref="F13">_xlfn.XLOOKUP($A13,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>2675 BL</v>
+      </c>
+      <c r="G13" t="str" cm="1">
+        <f t="array" ref="G13">_xlfn.XLOOKUP($A13,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Honselersdijk</v>
+      </c>
+      <c r="H13" t="str" cm="1">
+        <f t="array" ref="H13">_xlfn.XLOOKUP($A13,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-51611737 Barbara / 06-54398790 Maup</v>
+      </c>
+      <c r="I13" t="str" cm="1">
+        <f t="array" ref="I13">_xlfn.XLOOKUP($A13,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>endem3@caiway.nl</v>
+      </c>
+      <c r="J13" t="str" cm="1">
+        <f t="array" ref="J13">_xlfn.XLOOKUP($A13,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL81INGB0112509347</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="49">
+        <v>282</v>
+      </c>
+      <c r="B14" cm="1">
+        <f t="array" ref="B14">_xlfn.XLOOKUP($A14,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>0</v>
+      </c>
+      <c r="C14" t="str" cm="1">
+        <f t="array" ref="C14">_xlfn.XLOOKUP($A14,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>H. van Leeuwen</v>
+      </c>
+      <c r="D14" t="str" cm="1">
+        <f t="array" ref="D14">_xlfn.XLOOKUP($A14,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>Petra</v>
+      </c>
+      <c r="E14" t="str" cm="1">
+        <f t="array" ref="E14">_xlfn.XLOOKUP($A14,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Postbus 170</v>
+      </c>
+      <c r="F14" t="str" cm="1">
+        <f t="array" ref="F14">_xlfn.XLOOKUP($A14,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>2680 AD</v>
+      </c>
+      <c r="G14" t="str" cm="1">
+        <f t="array" ref="G14">_xlfn.XLOOKUP($A14,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Monster</v>
+      </c>
+      <c r="H14" t="str" cm="1">
+        <f t="array" ref="H14">_xlfn.XLOOKUP($A14,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-51262904 / 0174-248804</v>
+      </c>
+      <c r="I14" t="str" cm="1">
+        <f t="array" ref="I14">_xlfn.XLOOKUP($A14,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>petra@huubvanleeuwen.nl</v>
+      </c>
+      <c r="J14" t="str" cm="1">
+        <f t="array" ref="J14">_xlfn.XLOOKUP($A14,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL96RABO0375644504</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="50">
+        <v>283</v>
+      </c>
+      <c r="B15" cm="1">
+        <f t="array" ref="B15">_xlfn.XLOOKUP($A15,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>632.86999999999989</v>
+      </c>
+      <c r="C15" t="str" cm="1">
+        <f t="array" ref="C15">_xlfn.XLOOKUP($A15,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>J.S. Vink Vastgoed</v>
+      </c>
+      <c r="D15" t="str" cm="1">
+        <f t="array" ref="D15">_xlfn.XLOOKUP($A15,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>Denise Vink</v>
+      </c>
+      <c r="E15" t="str" cm="1">
+        <f t="array" ref="E15">_xlfn.XLOOKUP($A15,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Boomaweg 27</v>
+      </c>
+      <c r="F15" t="str" cm="1">
+        <f t="array" ref="F15">_xlfn.XLOOKUP($A15,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v xml:space="preserve">2681 RH </v>
+      </c>
+      <c r="G15" t="str" cm="1">
+        <f t="array" ref="G15">_xlfn.XLOOKUP($A15,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Monster</v>
+      </c>
+      <c r="H15" t="str" cm="1">
+        <f t="array" ref="H15">_xlfn.XLOOKUP($A15,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-23615767 (denise) 06-53505331 (jan)</v>
+      </c>
+      <c r="I15" t="str" cm="1">
+        <f t="array" ref="I15">_xlfn.XLOOKUP($A15,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>info@jsvink.nl / d.j.vink@hotmail.com</v>
+      </c>
+      <c r="J15" t="str" cm="1">
+        <f t="array" ref="J15">_xlfn.XLOOKUP($A15,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL14RABO3291687140 en NL20RABO0129949140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="49">
+        <v>285</v>
+      </c>
+      <c r="B16" cm="1">
+        <f t="array" ref="B16">_xlfn.XLOOKUP($A16,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>0</v>
+      </c>
+      <c r="C16" t="str" cm="1">
+        <f t="array" ref="C16">_xlfn.XLOOKUP($A16,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>P.C. Vijverberg</v>
+      </c>
+      <c r="D16" t="str" cm="1">
+        <f t="array" ref="D16">_xlfn.XLOOKUP($A16,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>Piet Vijverberg</v>
+      </c>
+      <c r="E16" t="str" cm="1">
+        <f t="array" ref="E16">_xlfn.XLOOKUP($A16,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Van Koppenweg 24</v>
+      </c>
+      <c r="F16" t="str" cm="1">
+        <f t="array" ref="F16">_xlfn.XLOOKUP($A16,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>2672 EH</v>
+      </c>
+      <c r="G16" t="str" cm="1">
+        <f t="array" ref="G16">_xlfn.XLOOKUP($A16,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Naaldwijk</v>
+      </c>
+      <c r="H16" t="str" cm="1">
+        <f t="array" ref="H16">_xlfn.XLOOKUP($A16,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-53299575</v>
+      </c>
+      <c r="I16" t="str" cm="1">
+        <f t="array" ref="I16">_xlfn.XLOOKUP($A16,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>piet@pietvijverberg.nl</v>
+      </c>
+      <c r="J16" t="str" cm="1">
+        <f t="array" ref="J16">_xlfn.XLOOKUP($A16,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL95RABO0142277460</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="50">
+        <v>378</v>
+      </c>
+      <c r="B17" cm="1">
+        <f t="array" ref="B17">_xlfn.XLOOKUP($A17,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>0</v>
+      </c>
+      <c r="C17" t="str" cm="1">
+        <f t="array" ref="C17">_xlfn.XLOOKUP($A17,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>P.C. Vijverberg</v>
+      </c>
+      <c r="D17" t="str" cm="1">
+        <f t="array" ref="D17">_xlfn.XLOOKUP($A17,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>Piet Vijverberg</v>
+      </c>
+      <c r="E17" t="str" cm="1">
+        <f t="array" ref="E17">_xlfn.XLOOKUP($A17,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Van Koppenweg 24</v>
+      </c>
+      <c r="F17" t="str" cm="1">
+        <f t="array" ref="F17">_xlfn.XLOOKUP($A17,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>2672 EH</v>
+      </c>
+      <c r="G17" t="str" cm="1">
+        <f t="array" ref="G17">_xlfn.XLOOKUP($A17,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Naaldwijk</v>
+      </c>
+      <c r="H17" t="str" cm="1">
+        <f t="array" ref="H17">_xlfn.XLOOKUP($A17,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-53299575</v>
+      </c>
+      <c r="I17" t="str" cm="1">
+        <f t="array" ref="I17">_xlfn.XLOOKUP($A17,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>piet@pietvijverberg.nl</v>
+      </c>
+      <c r="J17" t="str" cm="1">
+        <f t="array" ref="J17">_xlfn.XLOOKUP($A17,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL95RABO0142277460</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="50">
+        <v>363</v>
+      </c>
+      <c r="B18" cm="1">
+        <f t="array" ref="B18">_xlfn.XLOOKUP($A18,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>6.7</v>
+      </c>
+      <c r="C18" t="str" cm="1">
+        <f t="array" ref="C18">_xlfn.XLOOKUP($A18,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>S.A. van Bergen Vastgoed B.V.</v>
+      </c>
+      <c r="D18" t="str" cm="1">
+        <f t="array" ref="D18">_xlfn.XLOOKUP($A18,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>S.A. van Bergen</v>
+      </c>
+      <c r="E18" t="str" cm="1">
+        <f t="array" ref="E18">_xlfn.XLOOKUP($A18,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Strandweg 25</v>
+      </c>
+      <c r="F18" t="str" cm="1">
+        <f t="array" ref="F18">_xlfn.XLOOKUP($A18,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>3151 HV</v>
+      </c>
+      <c r="G18" t="str" cm="1">
+        <f t="array" ref="G18">_xlfn.XLOOKUP($A18,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Hoek van holland</v>
+      </c>
+      <c r="H18" t="str" cm="1">
+        <f t="array" ref="H18">_xlfn.XLOOKUP($A18,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-30412153</v>
+      </c>
+      <c r="I18" t="str" cm="1">
+        <f t="array" ref="I18">_xlfn.XLOOKUP($A18,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>bas.vanbergen@aubvanbergen.nl</v>
+      </c>
+      <c r="J18" t="str" cm="1">
+        <f t="array" ref="J18">_xlfn.XLOOKUP($A18,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL11RABO0318502364</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="50">
+        <v>364</v>
+      </c>
+      <c r="B19" cm="1">
+        <f t="array" ref="B19">_xlfn.XLOOKUP($A19,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>6.7</v>
+      </c>
+      <c r="C19" t="str" cm="1">
+        <f t="array" ref="C19">_xlfn.XLOOKUP($A19,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>S.A. van Bergen Vastgoed B.V.</v>
+      </c>
+      <c r="D19" t="str" cm="1">
+        <f t="array" ref="D19">_xlfn.XLOOKUP($A19,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>S.A. van Bergen</v>
+      </c>
+      <c r="E19" t="str" cm="1">
+        <f t="array" ref="E19">_xlfn.XLOOKUP($A19,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Strandweg 25</v>
+      </c>
+      <c r="F19" t="str" cm="1">
+        <f t="array" ref="F19">_xlfn.XLOOKUP($A19,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>3151 HV</v>
+      </c>
+      <c r="G19" t="str" cm="1">
+        <f t="array" ref="G19">_xlfn.XLOOKUP($A19,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Hoek van holland</v>
+      </c>
+      <c r="H19" t="str" cm="1">
+        <f t="array" ref="H19">_xlfn.XLOOKUP($A19,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-30412153</v>
+      </c>
+      <c r="I19" t="str" cm="1">
+        <f t="array" ref="I19">_xlfn.XLOOKUP($A19,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>bas.vanbergen@aubvanbergen.nl</v>
+      </c>
+      <c r="J19" t="str" cm="1">
+        <f t="array" ref="J19">_xlfn.XLOOKUP($A19,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL11RABO0318502364</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="50">
+        <v>377</v>
+      </c>
+      <c r="B20" cm="1">
+        <f t="array" ref="B20">_xlfn.XLOOKUP($A20,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>0</v>
+      </c>
+      <c r="C20" t="str" cm="1">
+        <f t="array" ref="C20">_xlfn.XLOOKUP($A20,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>F.A.S. van Bergen</v>
+      </c>
+      <c r="D20" t="str" cm="1">
+        <f t="array" ref="D20">_xlfn.XLOOKUP($A20,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>J. v. Bergen</v>
+      </c>
+      <c r="E20" t="str" cm="1">
+        <f t="array" ref="E20">_xlfn.XLOOKUP($A20,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Rijpstraat 22</v>
+      </c>
+      <c r="F20" t="str" cm="1">
+        <f t="array" ref="F20">_xlfn.XLOOKUP($A20,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>3151 BV</v>
+      </c>
+      <c r="G20" t="str" cm="1">
+        <f t="array" ref="G20">_xlfn.XLOOKUP($A20,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Hoek van Holland</v>
+      </c>
+      <c r="H20" t="str" cm="1">
+        <f t="array" ref="H20">_xlfn.XLOOKUP($A20,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-53739975</v>
+      </c>
+      <c r="I20" t="str" cm="1">
+        <f t="array" ref="I20">_xlfn.XLOOKUP($A20,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>jetvbergen@gmail.com</v>
+      </c>
+      <c r="J20" t="str" cm="1">
+        <f t="array" ref="J20">_xlfn.XLOOKUP($A20,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL44ABNA0620327766</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="49">
+        <v>286</v>
+      </c>
+      <c r="B21" cm="1">
+        <f t="array" ref="B21">_xlfn.XLOOKUP($A21,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>633.75999999999976</v>
+      </c>
+      <c r="C21" t="str" cm="1">
+        <f t="array" ref="C21">_xlfn.XLOOKUP($A21,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>T. Olsthoorn</v>
+      </c>
+      <c r="D21" t="str" cm="1">
+        <f t="array" ref="D21">_xlfn.XLOOKUP($A21,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>Ton Olsthoorn</v>
+      </c>
+      <c r="E21" t="str" cm="1">
+        <f t="array" ref="E21">_xlfn.XLOOKUP($A21,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Ravellaan 8</v>
+      </c>
+      <c r="F21" t="str" cm="1">
+        <f t="array" ref="F21">_xlfn.XLOOKUP($A21,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>2671 VT</v>
+      </c>
+      <c r="G21" t="str" cm="1">
+        <f t="array" ref="G21">_xlfn.XLOOKUP($A21,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Naaldwijk</v>
+      </c>
+      <c r="H21" t="str" cm="1">
+        <f t="array" ref="H21">_xlfn.XLOOKUP($A21,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-22413459</v>
+      </c>
+      <c r="I21" t="str" cm="1">
+        <f t="array" ref="I21">_xlfn.XLOOKUP($A21,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>tonolsthoorn@kpnmail.nl</v>
+      </c>
+      <c r="J21" t="str" cm="1">
+        <f t="array" ref="J21">_xlfn.XLOOKUP($A21,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL92RABO0342957031</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="50">
+        <v>288</v>
+      </c>
+      <c r="B22" cm="1">
+        <f t="array" ref="B22">_xlfn.XLOOKUP($A22,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>48.21</v>
+      </c>
+      <c r="C22" t="str" cm="1">
+        <f t="array" ref="C22">_xlfn.XLOOKUP($A22,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>Stichting MCM</v>
+      </c>
+      <c r="D22" t="str" cm="1">
+        <f t="array" ref="D22">_xlfn.XLOOKUP($A22,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>J. v. Bergen</v>
+      </c>
+      <c r="E22" t="str" cm="1">
+        <f t="array" ref="E22">_xlfn.XLOOKUP($A22,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Rijpstraat 22</v>
+      </c>
+      <c r="F22" t="str" cm="1">
+        <f t="array" ref="F22">_xlfn.XLOOKUP($A22,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>3151 BV</v>
+      </c>
+      <c r="G22" t="str" cm="1">
+        <f t="array" ref="G22">_xlfn.XLOOKUP($A22,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Hoek van Holland</v>
+      </c>
+      <c r="H22" t="str" cm="1">
+        <f t="array" ref="H22">_xlfn.XLOOKUP($A22,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-53739975</v>
+      </c>
+      <c r="I22" t="str" cm="1">
+        <f t="array" ref="I22">_xlfn.XLOOKUP($A22,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>jetvbergen@gmail.com</v>
+      </c>
+      <c r="J22" t="str" cm="1">
+        <f t="array" ref="J22">_xlfn.XLOOKUP($A22,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL39RABO0334435080</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="50">
+        <v>289</v>
+      </c>
+      <c r="B23" cm="1">
+        <f t="array" ref="B23">_xlfn.XLOOKUP($A23,1*Sheet1!$A:$A,Sheet1!AE:AE,"",0)</f>
+        <v>0</v>
+      </c>
+      <c r="C23" t="str" cm="1">
+        <f t="array" ref="C23">_xlfn.XLOOKUP($A23,1*Sheet1!$A:$A,Sheet1!F:F,"",0)</f>
+        <v>Stichting MCM</v>
+      </c>
+      <c r="D23" t="str" cm="1">
+        <f t="array" ref="D23">_xlfn.XLOOKUP($A23,1*Sheet1!$A:$A,Sheet1!G:G,"",0)</f>
+        <v>J. v. Bergen</v>
+      </c>
+      <c r="E23" t="str" cm="1">
+        <f t="array" ref="E23">_xlfn.XLOOKUP($A23,1*Sheet1!$A:$A,Sheet1!H:H,"",0)</f>
+        <v>Rijpstraat 22</v>
+      </c>
+      <c r="F23" t="str" cm="1">
+        <f t="array" ref="F23">_xlfn.XLOOKUP($A23,1*Sheet1!$A:$A,Sheet1!I:I,"",0)</f>
+        <v>3151 BV</v>
+      </c>
+      <c r="G23" t="str" cm="1">
+        <f t="array" ref="G23">_xlfn.XLOOKUP($A23,1*Sheet1!$A:$A,Sheet1!J:J,"",0)</f>
+        <v>Hoek van Holland</v>
+      </c>
+      <c r="H23" t="str" cm="1">
+        <f t="array" ref="H23">_xlfn.XLOOKUP($A23,1*Sheet1!$A:$A,Sheet1!K:K,"",0)</f>
+        <v>06-53739975</v>
+      </c>
+      <c r="I23" t="str" cm="1">
+        <f t="array" ref="I23">_xlfn.XLOOKUP($A23,1*Sheet1!$A:$A,Sheet1!L:L,"",0)</f>
+        <v>jetvbergen@gmail.com</v>
+      </c>
+      <c r="J23" t="str" cm="1">
+        <f t="array" ref="J23">_xlfn.XLOOKUP($A23,1*Sheet1!$A:$A,Sheet1!M:M,"",0)</f>
+        <v>NL39RABO0334435080</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD8216A3BCF59A4CAC1EDC9B65F03F94" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7a5dd83b0615c7ab65f6e497dc3f1a67">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2" xmlns:ns3="7c6541c9-858d-46cc-aee4-1fa681dc1bd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b3083ab368e81f90f854d4b93d60013" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD8216A3BCF59A4CAC1EDC9B65F03F94" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0e72e358fff385e948993b5140718f2">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2" xmlns:ns3="7c6541c9-858d-46cc-aee4-1fa681dc1bd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f2e1edef662b1e8a4a57019bf45cf5f9" ns2:_="" ns3:_="">
     <xsd:import namespace="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2"/>
     <xsd:import namespace="7c6541c9-858d-46cc-aee4-1fa681dc1bd6"/>
     <xsd:element name="properties">
@@ -4594,15 +5601,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2">
@@ -4613,14 +5611,40 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1B8B65B-90D4-4CFA-B64D-55ACEE3E0EDE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CE4D5A7-A065-486E-91FC-24386961D527}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F540105A-E155-4263-8FF1-0970CB25BEC5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58A0F90D-F385-44E4-8B91-56BDAB481306}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="7c6541c9-858d-46cc-aee4-1fa681dc1bd6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58A0F90D-F385-44E4-8B91-56BDAB481306}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F540105A-E155-4263-8FF1-0970CB25BEC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>